<commit_message>
Update excel file, sheet name and configuration.properties file.
</commit_message>
<xml_diff>
--- a/VyTrackQa2Users.xlsx
+++ b/VyTrackQa2Users.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aysundamar/IdeaProjects/ApcahePOI-practice/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8C6174-5479-FE44-929C-8FB5AF8E6A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27511"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{56B860DC-19D0-40CC-B83A-95C2CD02C4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="1700" windowWidth="21580" windowHeight="16440" xr2:uid="{47319A83-4017-A548-AEBB-A2F2B1387863}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VytrackUsers" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +22,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -63,57 +60,27 @@
     <t>user2</t>
   </si>
   <si>
-    <t>Bella</t>
-  </si>
-  <si>
-    <t>Stamm</t>
-  </si>
-  <si>
     <t>storemanager51</t>
   </si>
   <si>
-    <t>Edd</t>
-  </si>
-  <si>
-    <t>Turner</t>
-  </si>
-  <si>
     <t>storemanager52</t>
   </si>
   <si>
     <t>salesmanager101</t>
   </si>
   <si>
-    <t>Liza</t>
-  </si>
-  <si>
-    <t>Fritsch</t>
-  </si>
-  <si>
     <t>salesmanager102</t>
-  </si>
-  <si>
-    <t>Pierre</t>
-  </si>
-  <si>
-    <t>Prohaska</t>
-  </si>
-  <si>
-    <t>Roma</t>
-  </si>
-  <si>
-    <t>Medhurst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -145,7 +112,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -168,39 +135,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="145F82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="186C24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -252,7 +219,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -363,13 +330,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -378,6 +338,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -442,7 +409,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -453,22 +440,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45CC427-CF7F-3D44-80B5-6A431C042EC8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="214" zoomScaleNormal="214" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1" collapsed="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -496,7 +477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -504,66 +485,66 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>